<commit_message>
Alteração no backlog de requisitos + telas do site(login e cadastro concluídas)
</commit_message>
<xml_diff>
--- a/Documentação/BackLog de Requisitos - BornGothic.xlsx
+++ b/Documentação/BackLog de Requisitos - BornGothic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\OneDrive\Desktop\sptech-koga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\OneDrive\Desktop\sptech-koga\PROJETO PI\Born-Gothic-Projeto-Individual\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9784316C-EEC6-48B6-B330-BA12DF69F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69616E89-84FF-4BBF-AF07-2BEC098ADF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5616" yWindow="972" windowWidth="17280" windowHeight="10764" xr2:uid="{240B8422-38C4-410A-92FD-61370D50BED2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{240B8422-38C4-410A-92FD-61370D50BED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -508,20 +508,8 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -530,12 +518,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -550,28 +532,28 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -581,6 +563,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -748,16 +748,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>123</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.25</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.5</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.75</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -838,10 +838,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>123</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>58</c:v>
@@ -1668,10 +1668,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1993,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC8D886-CB9B-4AED-8453-F33DBF6EA1ED}">
   <dimension ref="D3:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="48" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2017,586 +2013,586 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="4:19" ht="27.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="N5" s="5" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="N5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="R5" s="6" t="s">
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="R5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="4:19" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="9">
         <v>8</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="9">
         <v>1</v>
       </c>
-      <c r="K6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" s="23" t="s">
+      <c r="K6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="O6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="P6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="R6" s="23">
+      <c r="R6" s="17">
         <v>1</v>
       </c>
-      <c r="S6" s="24">
-        <v>32</v>
+      <c r="S6" s="18">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="4:19" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="9">
         <v>5</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="9">
         <v>1</v>
       </c>
-      <c r="K7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="24">
+      <c r="K7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="18">
         <v>1</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="19">
         <v>45774</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="19">
         <v>45780</v>
       </c>
-      <c r="R7" s="23">
+      <c r="R7" s="17">
         <v>2</v>
       </c>
-      <c r="S7" s="24">
-        <v>33</v>
+      <c r="S7" s="18">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="4:19" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="9">
         <v>5</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="9">
         <v>1</v>
       </c>
-      <c r="K8" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="24">
+      <c r="K8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="18">
         <v>2</v>
       </c>
-      <c r="O8" s="25">
+      <c r="O8" s="19">
         <v>45781</v>
       </c>
-      <c r="P8" s="25">
+      <c r="P8" s="19">
         <v>45787</v>
       </c>
-      <c r="R8" s="23">
+      <c r="R8" s="17">
         <v>3</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="18">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="4:19" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="9">
         <v>5</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="9">
         <v>1</v>
       </c>
-      <c r="K9" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="N9" s="24">
+      <c r="K9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="18">
         <v>3</v>
       </c>
-      <c r="O9" s="25">
+      <c r="O9" s="19">
         <v>45788</v>
       </c>
-      <c r="P9" s="25">
+      <c r="P9" s="19">
         <v>45794</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="17">
         <v>4</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="18">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="4:19" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="9">
         <v>5</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="9">
         <v>1</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="18">
         <v>4</v>
       </c>
-      <c r="O10" s="25">
+      <c r="O10" s="19">
         <v>45795</v>
       </c>
-      <c r="P10" s="25">
+      <c r="P10" s="19">
         <v>45801</v>
       </c>
     </row>
     <row r="11" spans="4:19" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="9">
         <v>13</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="9">
         <v>1</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="4:19" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="9">
         <v>13</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="9">
         <v>1</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="4:19" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="9">
         <v>8</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="9">
         <v>2</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="O13" s="10"/>
-      <c r="P13" s="11" t="s">
+      <c r="O13" s="22"/>
+      <c r="P13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Q13" s="12" t="s">
+      <c r="Q13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="R13" s="13" t="s">
+      <c r="R13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="S13" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="14" spans="4:19" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="9">
         <v>8</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="9">
         <v>2</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="N14" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="O14" s="7">
-        <v>123</v>
-      </c>
-      <c r="P14" s="8">
-        <v>92.25</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>61.5</v>
-      </c>
-      <c r="R14" s="8">
-        <v>30.75</v>
-      </c>
-      <c r="S14" s="8">
+      <c r="O14" s="3">
+        <v>120</v>
+      </c>
+      <c r="P14" s="4">
+        <v>90</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>60</v>
+      </c>
+      <c r="R14" s="4">
+        <v>30</v>
+      </c>
+      <c r="S14" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="4:19" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="9">
         <v>8</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="N15" s="14" t="s">
+      <c r="N15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="O15" s="7">
-        <v>123</v>
-      </c>
-      <c r="P15" s="8">
-        <v>91</v>
-      </c>
-      <c r="Q15" s="8">
+      <c r="O15" s="3">
+        <v>120</v>
+      </c>
+      <c r="P15" s="4">
+        <v>92</v>
+      </c>
+      <c r="Q15" s="4">
         <v>58</v>
       </c>
-      <c r="R15" s="8">
+      <c r="R15" s="4">
         <v>24</v>
       </c>
-      <c r="S15" s="8">
+      <c r="S15" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="4:19" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="4:11" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="13">
         <v>8</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="13">
         <v>1</v>
       </c>
-      <c r="K17" s="19" t="s">
-        <v>7</v>
+      <c r="K17" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="4:11" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="9">
         <v>13</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="9">
         <v>1</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="4:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="9">
         <v>8</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="4:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="15">
-        <v>8</v>
-      </c>
-      <c r="J20" s="15">
+      <c r="H20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="9">
+        <v>5</v>
+      </c>
+      <c r="J20" s="9">
         <v>1</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="4:11" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="9">
         <v>8</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="9">
         <v>1</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="K21" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2620,6 +2616,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045B33021656A9E479DF12B9A8EE42828" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5ede22190f62034867da76e552493950">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1dc861b8-2196-455d-b291-a999da8cffb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7b92c7a709487a617ea736db7e12b693" ns3:_="">
     <xsd:import namespace="1dc861b8-2196-455d-b291-a999da8cffb6"/>
@@ -2801,15 +2806,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2819,6 +2815,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{879ABC2B-24C8-42D6-A379-5D9E812A53A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B1DD218-DDF4-49B7-912F-990F90DABBF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2832,14 +2836,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{879ABC2B-24C8-42D6-A379-5D9E812A53A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Início da página principal do site + alteração no backlog de requisitos
</commit_message>
<xml_diff>
--- a/Documentação/BackLog de Requisitos - BornGothic.xlsx
+++ b/Documentação/BackLog de Requisitos - BornGothic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\OneDrive\Desktop\sptech-koga\PROJETO PI\Born-Gothic-Projeto-Individual\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69616E89-84FF-4BBF-AF07-2BEC098ADF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5B75B4-61B2-4AED-9766-C2C514B602D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{240B8422-38C4-410A-92FD-61370D50BED2}"/>
   </bookViews>
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC8D886-CB9B-4AED-8453-F33DBF6EA1ED}">
   <dimension ref="D3:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2616,12 +2616,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1dc861b8-2196-455d-b291-a999da8cffb6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2807,17 +2806,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1dc861b8-2196-455d-b291-a999da8cffb6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{879ABC2B-24C8-42D6-A379-5D9E812A53A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3D11105-804D-4A81-A790-2E376BAD8F22}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1dc861b8-2196-455d-b291-a999da8cffb6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2841,17 +2849,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3D11105-804D-4A81-A790-2E376BAD8F22}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{879ABC2B-24C8-42D6-A379-5D9E812A53A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1dc861b8-2196-455d-b291-a999da8cffb6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>